<commit_message>
EDSF-75: Adding ability to set number of projected cash flow periods based off of last lagged warranty payment
</commit_message>
<xml_diff>
--- a/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
+++ b/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.Core.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABED41-1DFB-4BCF-87C5-AE3799DD1B80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940AE677-D70E-4657-95C5-169E8397745B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="765" windowWidth="16080" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="30" windowWidth="9885" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NCES Data By Major'!$C$2:$F$155</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Scenarios!$B$2:$Z$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Scenarios!$B$2:$AB$12</definedName>
     <definedName name="Assumptions_TargetEnd_Scenario2">'[1]Assumptions - Dropouts'!$F$4</definedName>
     <definedName name="Assumptions_TargetEnd_Scenario3">'[1]Assumptions - Dropouts'!$F$5</definedName>
     <definedName name="Assumptions_TargetEnd_Scenario4">'[1]Assumptions - Dropouts'!$F$6</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="232">
   <si>
     <t>Scenario</t>
   </si>
@@ -744,6 +744,12 @@
   </si>
   <si>
     <t>Margin</t>
+  </si>
+  <si>
+    <t>WarrantyLagMonths</t>
+  </si>
+  <si>
+    <t>WarrantyRepayMonths</t>
   </si>
 </sst>
 </file>
@@ -937,7 +943,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1063,6 +1069,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1460,14 +1469,14 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B2:Z12"/>
+  <dimension ref="B2:AB12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,13 +1502,15 @@
     <col min="19" max="19" width="23.140625" customWidth="1"/>
     <col min="20" max="20" width="17.140625" customWidth="1"/>
     <col min="21" max="21" width="24.42578125" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.28515625" customWidth="1"/>
+    <col min="23" max="23" width="22.5703125" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
@@ -1560,23 +1571,29 @@
       <c r="U2" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="W2" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="X2" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="27" t="s">
+      <c r="Z2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1641,23 +1658,29 @@
       <c r="U3" s="28">
         <v>0</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="28">
+        <v>0</v>
+      </c>
+      <c r="W3" s="28">
+        <v>0</v>
+      </c>
+      <c r="X3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="Y3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="8">
+      <c r="Z3" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
         <f>B3+1</f>
         <v>2</v>
@@ -1723,23 +1746,29 @@
       <c r="U4" s="28">
         <v>0</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="28">
+        <v>0</v>
+      </c>
+      <c r="W4" s="28">
+        <v>0</v>
+      </c>
+      <c r="X4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W4" s="15" t="s">
+      <c r="Y4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X4" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="8">
+      <c r="Z4" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <f t="shared" ref="B5:B12" si="4">B4+1</f>
         <v>3</v>
@@ -1805,23 +1834,29 @@
       <c r="U5" s="28">
         <v>0</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="V5" s="28">
+        <v>0</v>
+      </c>
+      <c r="W5" s="28">
+        <v>0</v>
+      </c>
+      <c r="X5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W5" s="15" t="s">
+      <c r="Y5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X5" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="8">
+      <c r="Z5" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -1887,23 +1922,29 @@
       <c r="U6" s="28">
         <v>0</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="28">
+        <v>0</v>
+      </c>
+      <c r="W6" s="28">
+        <v>0</v>
+      </c>
+      <c r="X6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="Y6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X6" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="8">
+      <c r="Z6" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -1969,23 +2010,29 @@
       <c r="U7" s="28">
         <v>0</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="28">
+        <v>0</v>
+      </c>
+      <c r="W7" s="28">
+        <v>0</v>
+      </c>
+      <c r="X7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W7" s="15" t="s">
+      <c r="Y7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="8">
+      <c r="Z7" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -2051,23 +2098,29 @@
       <c r="U8" s="28">
         <v>0</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="V8" s="28">
+        <v>0</v>
+      </c>
+      <c r="W8" s="28">
+        <v>0</v>
+      </c>
+      <c r="X8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="Y8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X8" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="8">
+      <c r="Z8" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="44">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2131,23 +2184,29 @@
       <c r="U9" s="54">
         <v>12</v>
       </c>
-      <c r="V9" s="55" t="s">
+      <c r="V9" s="54">
+        <v>0</v>
+      </c>
+      <c r="W9" s="54">
+        <v>0</v>
+      </c>
+      <c r="X9" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="W9" s="55" t="s">
+      <c r="Y9" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="X9" s="54">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="56">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="57">
+      <c r="Z9" s="54">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="57">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -2156,80 +2215,84 @@
         <v>64</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>228</v>
       </c>
       <c r="F10" s="42">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G10" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H10" s="42">
         <v>0.25</v>
       </c>
       <c r="I10" s="42">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="J10" s="42">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="K10" s="29">
-        <v>14.5079231933478</v>
+        <v>15</v>
       </c>
       <c r="L10" s="30">
-        <v>4.4493882091212456</v>
+        <v>10</v>
       </c>
       <c r="M10" s="29">
-        <v>1.8745783110559984</v>
+        <v>5</v>
       </c>
       <c r="N10" s="31">
         <f t="shared" si="5"/>
-        <v>79.168110286474956</v>
+        <v>70</v>
       </c>
       <c r="O10" s="9">
         <f t="shared" si="6"/>
-        <v>10.231889713525042</v>
+        <v>21</v>
       </c>
       <c r="P10" s="2">
         <v>0</v>
       </c>
       <c r="Q10" s="32">
-        <f>MIN(('NCES Data By Major'!D10+'NCES Data By Major'!E10)*100,
-100-(N10+P10+G10))</f>
-        <v>5.6000000000000005</v>
+        <v>9</v>
       </c>
       <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="28">
+        <v>0</v>
+      </c>
+      <c r="T10" s="28">
+        <v>3078.0607400833542</v>
+      </c>
+      <c r="U10" s="28">
+        <v>12</v>
+      </c>
+      <c r="V10" s="28">
+        <v>6</v>
+      </c>
+      <c r="W10" s="28">
+        <v>36</v>
+      </c>
+      <c r="X10" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="S10" s="28">
-        <v>10250</v>
-      </c>
-      <c r="T10" s="28">
-        <v>0</v>
-      </c>
-      <c r="U10" s="28">
-        <v>0</v>
-      </c>
-      <c r="V10" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="W10" s="15" t="s">
+      <c r="Y10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X10" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="8">
+      <c r="Z10" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -2295,23 +2358,29 @@
       <c r="U11" s="28">
         <v>0</v>
       </c>
-      <c r="V11" s="15" t="s">
+      <c r="V11" s="28">
+        <v>0</v>
+      </c>
+      <c r="W11" s="28">
+        <v>0</v>
+      </c>
+      <c r="X11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="Y11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X11" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="8">
+      <c r="Z11" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="8">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2377,26 +2446,32 @@
       <c r="U12" s="28">
         <v>0</v>
       </c>
-      <c r="V12" s="15" t="s">
+      <c r="V12" s="28">
+        <v>0</v>
+      </c>
+      <c r="W12" s="28">
+        <v>0</v>
+      </c>
+      <c r="X12" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W12" s="15" t="s">
+      <c r="Y12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X12" s="28">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="8">
+      <c r="Z12" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="8">
         <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:Z12" xr:uid="{41D0623F-35E4-467D-8335-5335D24492F3}"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W12" xr:uid="{3EE6BC6F-6AD2-4260-AAC6-BB0AE485DC9E}">
+  <autoFilter ref="B2:AB12" xr:uid="{41D0623F-35E4-467D-8335-5335D24492F3}"/>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y12" xr:uid="{3EE6BC6F-6AD2-4260-AAC6-BB0AE485DC9E}">
       <formula1>InterestRateTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -5341,7 +5416,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EDSF-75: Finished creating ability to spread and lag drop-out warranty payments, tied-out with Excel Model v.15
</commit_message>
<xml_diff>
--- a/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
+++ b/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.Core.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940AE677-D70E-4657-95C5-169E8397745B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410DC2E9-39E7-41FD-9C11-ED29FB1B29D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="30" windowWidth="9885" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="233">
   <si>
     <t>Scenario</t>
   </si>
@@ -750,6 +750,9 @@
   </si>
   <si>
     <t>WarrantyRepayMonths</t>
+  </si>
+  <si>
+    <t>WarrantyOnly</t>
   </si>
 </sst>
 </file>
@@ -814,7 +817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,8 +836,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -937,13 +946,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1072,6 +1103,54 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1472,11 +1551,11 @@
   <dimension ref="B2:AB12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,177 +2286,175 @@
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+      <c r="B10" s="63">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="F10" s="42">
+      <c r="E10" s="64" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" s="65">
         <v>0.15</v>
       </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="42">
+      <c r="G10" s="66">
+        <v>0</v>
+      </c>
+      <c r="H10" s="65">
+        <v>0</v>
+      </c>
+      <c r="I10" s="65">
         <v>0.25</v>
       </c>
-      <c r="I10" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="29">
+      <c r="J10" s="65">
+        <v>0</v>
+      </c>
+      <c r="K10" s="67">
         <v>15</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="68">
         <v>10</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="67">
         <v>5</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="51">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="52">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="32">
+      <c r="P10" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="53">
         <v>9</v>
       </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
-      <c r="S10" s="28">
-        <v>0</v>
-      </c>
-      <c r="T10" s="28">
+      <c r="R10" s="66">
+        <v>0</v>
+      </c>
+      <c r="S10" s="54">
+        <v>0</v>
+      </c>
+      <c r="T10" s="54">
         <v>3078.0607400833542</v>
       </c>
-      <c r="U10" s="28">
+      <c r="U10" s="54">
         <v>12</v>
       </c>
-      <c r="V10" s="28">
+      <c r="V10" s="54">
         <v>6</v>
       </c>
-      <c r="W10" s="28">
+      <c r="W10" s="54">
         <v>36</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="X10" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="Y10" s="15" t="s">
+      <c r="Y10" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="Z10" s="28">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="8">
+      <c r="Z10" s="54">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="75">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="76">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
+      <c r="B11" s="69">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="42">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5</v>
-      </c>
-      <c r="H11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I11" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="K11" s="29">
-        <v>14.5079231933478</v>
-      </c>
-      <c r="L11" s="30">
-        <v>4.4493882091212456</v>
-      </c>
-      <c r="M11" s="29">
-        <v>1.8745783110559984</v>
-      </c>
-      <c r="N11" s="31">
+      <c r="D11" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>232</v>
+      </c>
+      <c r="F11" s="71">
+        <v>0.15</v>
+      </c>
+      <c r="G11" s="72">
+        <v>0</v>
+      </c>
+      <c r="H11" s="71">
+        <v>0</v>
+      </c>
+      <c r="I11" s="71">
+        <v>0</v>
+      </c>
+      <c r="J11" s="71">
+        <v>0</v>
+      </c>
+      <c r="K11" s="73">
+        <v>50.354716363739897</v>
+      </c>
+      <c r="L11" s="74">
+        <v>0</v>
+      </c>
+      <c r="M11" s="73">
+        <v>0</v>
+      </c>
+      <c r="N11" s="59">
         <f t="shared" si="5"/>
-        <v>79.168110286474956</v>
-      </c>
-      <c r="O11" s="9">
+        <v>49.645283636260103</v>
+      </c>
+      <c r="O11" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="32">
-        <f>MIN(('NCES Data By Major'!D11+'NCES Data By Major'!E11)*100,
-100-(N11+P11+G11))</f>
-        <v>15.831889713525044</v>
-      </c>
-      <c r="R11" s="2">
+      <c r="P11" s="72">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="61">
+        <v>50.354716363739897</v>
+      </c>
+      <c r="R11" s="72">
+        <v>0</v>
+      </c>
+      <c r="S11" s="62">
+        <v>0</v>
+      </c>
+      <c r="T11" s="62">
+        <v>3078.0607400833542</v>
+      </c>
+      <c r="U11" s="62">
+        <v>24</v>
+      </c>
+      <c r="V11" s="62">
+        <v>6</v>
+      </c>
+      <c r="W11" s="62">
+        <v>36</v>
+      </c>
+      <c r="X11" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="28">
-        <v>12500</v>
-      </c>
-      <c r="T11" s="28">
-        <v>0</v>
-      </c>
-      <c r="U11" s="28">
-        <v>0</v>
-      </c>
-      <c r="V11" s="28">
-        <v>0</v>
-      </c>
-      <c r="W11" s="28">
-        <v>0</v>
-      </c>
-      <c r="X11" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y11" s="15" t="s">
+      <c r="Y11" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="Z11" s="28">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="8">
-        <v>72</v>
+      <c r="Z11" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="77">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="78">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
@@ -2470,7 +2547,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B2:AB12" xr:uid="{41D0623F-35E4-467D-8335-5335D24492F3}"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y12" xr:uid="{3EE6BC6F-6AD2-4260-AAC6-BB0AE485DC9E}">
       <formula1>InterestRateTypes</formula1>
     </dataValidation>
@@ -5133,10 +5210,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5398,9 +5475,80 @@
         <v>40</v>
       </c>
     </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="7">
+        <v>25</v>
+      </c>
+      <c r="E19" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7">
+        <v>25</v>
+      </c>
+      <c r="E20" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="7">
+        <v>10</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="7">
+        <v>40</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F18" xr:uid="{9E905705-5702-43B9-B10E-FBFFBDC727FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F23" xr:uid="{9E905705-5702-43B9-B10E-FBFFBDC727FD}">
       <formula1>EventTypes</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
EDSF-75: Added an "EndingPeriod" option for the costs and fees model
</commit_message>
<xml_diff>
--- a/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
+++ b/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.Core.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410DC2E9-39E7-41FD-9C11-ED29FB1B29D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CDCF69-459C-48B2-9758-6C45BFDE9509}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="235">
   <si>
     <t>Scenario</t>
   </si>
@@ -753,6 +753,12 @@
   </si>
   <si>
     <t>WarrantyOnly</t>
+  </si>
+  <si>
+    <t>EndingPeriod</t>
+  </si>
+  <si>
+    <t>NoDropOutRepay</t>
   </si>
 </sst>
 </file>
@@ -1551,11 +1557,11 @@
   <dimension ref="B2:AB12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,11 +1892,11 @@
         <v>1.8745783110559984</v>
       </c>
       <c r="N5" s="31">
-        <f t="shared" ref="N5:N12" si="5">100-SUM(K5:M5)</f>
+        <f t="shared" ref="N5:N11" si="5">100-SUM(K5:M5)</f>
         <v>79.168110286474956</v>
       </c>
       <c r="O5" s="9">
-        <f t="shared" ref="O5:O12" si="6">100-N5-SUM(P5:Q5)-G5</f>
+        <f t="shared" ref="O5:O11" si="6">100-N5-SUM(P5:Q5)-G5</f>
         <v>11.331889713525044</v>
       </c>
       <c r="P5" s="2">
@@ -2112,90 +2118,88 @@
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="B8" s="44">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="F8" s="42">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="D8" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F8" s="47">
+        <v>0.15</v>
+      </c>
+      <c r="G8" s="48">
+        <v>0</v>
+      </c>
+      <c r="H8" s="47">
+        <v>0</v>
+      </c>
+      <c r="I8" s="47">
+        <v>0</v>
+      </c>
+      <c r="J8" s="47">
+        <v>0</v>
+      </c>
+      <c r="K8" s="49">
+        <v>15</v>
+      </c>
+      <c r="L8" s="50">
+        <v>10</v>
+      </c>
+      <c r="M8" s="49">
         <v>5</v>
       </c>
-      <c r="H8" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I8" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="K8" s="29">
-        <v>14.5079231933478</v>
-      </c>
-      <c r="L8" s="30">
-        <v>4.4493882091212456</v>
-      </c>
-      <c r="M8" s="29">
-        <v>1.8745783110559984</v>
-      </c>
-      <c r="N8" s="31">
-        <f t="shared" si="5"/>
-        <v>79.168110286474956</v>
-      </c>
-      <c r="O8" s="9">
-        <f t="shared" si="6"/>
-        <v>10.231889713525042</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="32">
-        <f>MIN(('NCES Data By Major'!D8+'NCES Data By Major'!E8)*100,
-100-(N8+P8+G8))</f>
-        <v>5.6000000000000005</v>
-      </c>
-      <c r="R8" s="2">
+      <c r="N8" s="51">
+        <f t="shared" ref="N8" si="7">100-SUM(K8:M8)</f>
+        <v>70</v>
+      </c>
+      <c r="O8" s="52">
+        <f t="shared" ref="O8" si="8">100-N8-SUM(P8:Q8)-G8</f>
+        <v>21</v>
+      </c>
+      <c r="P8" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="53">
+        <v>9</v>
+      </c>
+      <c r="R8" s="48">
+        <v>0</v>
+      </c>
+      <c r="S8" s="54">
+        <v>4104.0809867778062</v>
+      </c>
+      <c r="T8" s="54">
+        <v>3078.0607400833542</v>
+      </c>
+      <c r="U8" s="54">
+        <v>12</v>
+      </c>
+      <c r="V8" s="54">
+        <v>6</v>
+      </c>
+      <c r="W8" s="54">
+        <v>36</v>
+      </c>
+      <c r="X8" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="S8" s="28">
-        <v>10250</v>
-      </c>
-      <c r="T8" s="28">
-        <v>0</v>
-      </c>
-      <c r="U8" s="28">
-        <v>0</v>
-      </c>
-      <c r="V8" s="28">
-        <v>0</v>
-      </c>
-      <c r="W8" s="28">
-        <v>0</v>
-      </c>
-      <c r="X8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y8" s="15" t="s">
+      <c r="Y8" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="Z8" s="28">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="8">
+      <c r="Z8" s="54">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="57">
         <v>72</v>
       </c>
     </row>
@@ -2458,91 +2462,89 @@
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+      <c r="B12" s="69">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="F12" s="42">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="H12" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I12" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="J12" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="K12" s="29">
-        <v>14.5079231933478</v>
-      </c>
-      <c r="L12" s="30">
-        <v>4.4493882091212456</v>
-      </c>
-      <c r="M12" s="29">
-        <v>1.8745783110559984</v>
-      </c>
-      <c r="N12" s="31">
-        <f t="shared" si="5"/>
-        <v>79.168110286474956</v>
-      </c>
-      <c r="O12" s="9">
-        <f t="shared" si="6"/>
-        <v>10.231889713525042</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="32">
-        <f>MIN(('NCES Data By Major'!D12+'NCES Data By Major'!E12)*100,
-100-(N12+P12+G12))</f>
-        <v>5.6000000000000005</v>
-      </c>
-      <c r="R12" s="2">
+      <c r="D12" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" s="65">
+        <v>0.15</v>
+      </c>
+      <c r="G12" s="66">
+        <v>0</v>
+      </c>
+      <c r="H12" s="65">
+        <v>0</v>
+      </c>
+      <c r="I12" s="65">
+        <v>0</v>
+      </c>
+      <c r="J12" s="65">
+        <v>0</v>
+      </c>
+      <c r="K12" s="67">
+        <v>68.796481574253903</v>
+      </c>
+      <c r="L12" s="68">
+        <v>0</v>
+      </c>
+      <c r="M12" s="67">
+        <v>0</v>
+      </c>
+      <c r="N12" s="51">
+        <f t="shared" ref="N12" si="9">100-SUM(K12:M12)</f>
+        <v>31.203518425746097</v>
+      </c>
+      <c r="O12" s="52">
+        <f t="shared" ref="O12" si="10">100-N12-SUM(P12:Q12)-G12</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="53">
+        <v>68.796481574253903</v>
+      </c>
+      <c r="R12" s="66">
+        <v>0</v>
+      </c>
+      <c r="S12" s="54">
+        <v>0</v>
+      </c>
+      <c r="T12" s="54">
+        <v>3078.0607400833542</v>
+      </c>
+      <c r="U12" s="54">
+        <v>12</v>
+      </c>
+      <c r="V12" s="54">
+        <v>6</v>
+      </c>
+      <c r="W12" s="54">
+        <v>36</v>
+      </c>
+      <c r="X12" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="S12" s="28">
-        <v>10250</v>
-      </c>
-      <c r="T12" s="28">
-        <v>0</v>
-      </c>
-      <c r="U12" s="28">
-        <v>0</v>
-      </c>
-      <c r="V12" s="28">
-        <v>0</v>
-      </c>
-      <c r="W12" s="28">
-        <v>0</v>
-      </c>
-      <c r="X12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y12" s="15" t="s">
+      <c r="Y12" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="Z12" s="28">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="8">
-        <v>72</v>
+      <c r="Z12" s="54">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="75">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="76">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5210,23 +5212,24 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>226</v>
       </c>
@@ -5242,8 +5245,11 @@
       <c r="F2" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>227</v>
       </c>
@@ -5257,7 +5263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>227</v>
       </c>
@@ -5271,7 +5277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>227</v>
       </c>
@@ -5285,7 +5291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>227</v>
       </c>
@@ -5299,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>227</v>
       </c>
@@ -5314,7 +5320,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>227</v>
       </c>
@@ -5329,7 +5335,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>227</v>
       </c>
@@ -5344,7 +5350,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>227</v>
       </c>
@@ -5359,23 +5365,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="7">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E11" s="10">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -5387,52 +5393,55 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E13" s="10">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="7">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -5447,7 +5456,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -5462,7 +5471,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C18" t="s">
         <v>36</v>
@@ -5477,13 +5486,13 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E19" s="10">
         <v>12</v>
@@ -5491,7 +5500,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
@@ -5505,13 +5514,13 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E21" s="10">
         <v>12</v>
@@ -5519,13 +5528,13 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E22" s="10">
         <v>1</v>
@@ -5533,22 +5542,138 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="7">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="7">
+        <v>150</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="7">
+        <v>300</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="7">
+        <v>25</v>
+      </c>
+      <c r="E27" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="7">
+        <v>25</v>
+      </c>
+      <c r="E28" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="7">
+        <v>10</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="7">
+        <v>40</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F23" xr:uid="{9E905705-5702-43B9-B10E-FBFFBDC727FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F31" xr:uid="{9E905705-5702-43B9-B10E-FBFFBDC727FD}">
       <formula1>EventTypes</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Building out institutions home page of the web site and web API
</commit_message>
<xml_diff>
--- a/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
+++ b/EduSafe.Core.Tests/Resources/EduSafe-Website-For-Profit-Scenario-Testing-Small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.Core.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CDCF69-459C-48B2-9758-6C45BFDE9509}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653E9381-4868-4BA1-81D0-C126D2BE4AFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1545" yWindow="420" windowWidth="16215" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -1561,7 +1561,7 @@
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="X9" sqref="X9"/>
+      <selection pane="bottomRight" activeCell="W2" sqref="V2:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>